<commit_message>
Update wa-2021 election file, make model text inputs wider
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-wa.xlsx
+++ b/python/Data/poll-data-wa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055EFCE1-46B6-4E7B-B0E7-ABC5B79E2797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B95630-15AE-440A-8A23-749CE8040D6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="-60" windowWidth="12030" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="4650" windowWidth="30180" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="17">
   <si>
     <t>MidDate</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>LIB FP</t>
+  </si>
+  <si>
+    <t>Painted Dog</t>
   </si>
 </sst>
 </file>
@@ -410,9 +413,9 @@
   <dimension ref="A1:U148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A43" activePane="bottomLeft"/>
       <selection activeCell="J1" sqref="J1:J1048576"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,6 +2758,35 @@
         <v>6</v>
       </c>
     </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71">
+        <v>66</v>
+      </c>
+      <c r="D71">
+        <v>21</v>
+      </c>
+      <c r="E71" s="6">
+        <v>49</v>
+      </c>
+      <c r="F71" s="6">
+        <v>13</v>
+      </c>
+      <c r="G71" s="6">
+        <v>7</v>
+      </c>
+      <c r="H71" s="6">
+        <v>4</v>
+      </c>
+      <c r="J71" s="6">
+        <v>6</v>
+      </c>
+    </row>
     <row r="118" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I118" s="5"/>
     </row>

</xml_diff>